<commit_message>
Ajout des informations relatives aux profits par livreurs
</commit_message>
<xml_diff>
--- a/media/izoua.xlsx
+++ b/media/izoua.xlsx
@@ -598,7 +598,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15 dÃ©cembre 2024</t>
+          <t>24 dÃ©cembre 2024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -608,17 +608,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Yoff</t>
+          <t>Ouest Foire</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>01h13</t>
+          <t>19h11</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Cagil</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Lahat Samb</t>
+          <t>Yves</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -638,17 +638,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Vosgienne Taille Grande, Vosgienne Taille Grande, Vosgienne Taille Grande</t>
+          <t>SELUCY Taille Grande, SELUCY - VOSGIENNE Taille Petite</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>7</v>
+        <v>1500</v>
       </c>
       <c r="K3" t="n">
-        <v>21000</v>
+        <v>8500</v>
       </c>
       <c r="L3" t="n">
-        <v>21007</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="4">

</xml_diff>